<commit_message>
adding metric functions, testing, and output plots
</commit_message>
<xml_diff>
--- a/data/processed/target_group_repo_ids.xlsx
+++ b/data/processed/target_group_repo_ids.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/paulsharratt/Documents/Hertie/Semester 4/03 - Master's Thesis/thesis_stf/data/processed/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FBC3C54-555D-FC43-8DE1-0B5FCC720769}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F7FA684-8A27-1C49-B38A-3748491F0979}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -509,10 +509,14 @@
   <dimension ref="A1:C23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+      <selection activeCell="A9" sqref="A9:B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="18.83203125" customWidth="1"/>
+    <col min="2" max="2" width="28" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">

</xml_diff>